<commit_message>
added getting data from spreadsheet for potluck cards and added 2 categories to spreadsheet. TODO: fill in rest of spreadsheet
</commit_message>
<xml_diff>
--- a/data/PropertyTycoonCardData.xlsx
+++ b/data/PropertyTycoonCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igor1\Desktop\project files\property-tycoon-38\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1567CC03-0CF2-4AA2-8CA4-659E99438A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B9E862-2171-4899-A702-4A29290ECE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BDE750ED-885A-4E53-AB7E-A47D1E3F79CA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BDE750ED-885A-4E53-AB7E-A47D1E3F79CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>Pot luck card data</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>Player token moves backwards to the Old Creek</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -558,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824FCAE1-2E2D-480B-8168-72B223ADDCE7}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,20 +577,26 @@
     <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -592,7 +604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -600,15 +612,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -616,7 +629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -624,7 +637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -632,7 +645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -640,7 +653,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -648,7 +661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -656,7 +669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -664,7 +677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -672,7 +685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -680,7 +693,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -731,10 +744,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699D9432-E6B2-493F-AA4E-F3BB0DC25130}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,20 +756,26 @@
     <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -764,7 +783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -772,7 +791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -780,7 +799,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
@@ -788,7 +807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -796,7 +815,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -804,7 +823,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
@@ -812,7 +831,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
@@ -820,7 +839,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -828,7 +847,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
@@ -836,7 +855,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>48</v>
       </c>
@@ -844,7 +863,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
@@ -852,7 +871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
@@ -886,5 +905,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more card types and also updated the spreadsheet
</commit_message>
<xml_diff>
--- a/data/PropertyTycoonCardData.xlsx
+++ b/data/PropertyTycoonCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igor1\Desktop\project files\property-tycoon-38\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B9E862-2171-4899-A702-4A29290ECE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8909F7-F028-4C16-B2D7-31B741A4217F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BDE750ED-885A-4E53-AB7E-A47D1E3F79CA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
   <si>
     <t>Pot luck card data</t>
   </si>
@@ -202,7 +202,37 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Amount</t>
+    <t>bpp</t>
+  </si>
+  <si>
+    <t>pm</t>
+  </si>
+  <si>
+    <t>ppb</t>
+  </si>
+  <si>
+    <t>ppp</t>
+  </si>
+  <si>
+    <t>ppf</t>
+  </si>
+  <si>
+    <t>pmf</t>
+  </si>
+  <si>
+    <t>pmx</t>
+  </si>
+  <si>
+    <t>ppr</t>
+  </si>
+  <si>
+    <t>jfc</t>
+  </si>
+  <si>
+    <t>HotelPrice</t>
+  </si>
+  <si>
+    <t>Amount/HousePice</t>
   </si>
 </sst>
 </file>
@@ -564,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824FCAE1-2E2D-480B-8168-72B223ADDCE7}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,14 +605,16 @@
     <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -593,147 +625,245 @@
         <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
     </row>
   </sheetData>
@@ -744,24 +874,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699D9432-E6B2-493F-AA4E-F3BB0DC25130}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -772,135 +904,222 @@
         <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed cards not getting the proper card type when reading from the spreadsheet
</commit_message>
<xml_diff>
--- a/data/PropertyTycoonCardData.xlsx
+++ b/data/PropertyTycoonCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igor1\Desktop\project files\property-tycoon-38\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8909F7-F028-4C16-B2D7-31B741A4217F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEACBFD-EB8B-4C56-9B61-3560DDE9048B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BDE750ED-885A-4E53-AB7E-A47D1E3F79CA}"/>
   </bookViews>
@@ -597,7 +597,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>